<commit_message>
Adicionado modo de abertura do google
</commit_message>
<xml_diff>
--- a/Agenda/agenda.xlsx
+++ b/Agenda/agenda.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesgranatyr/Documents/Ensino/IA Expert/Cursos/Assistente Virtual/curso_assistente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Pessoal\IA Expert\Assistente_Virtual\Agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A90D01-A057-1B44-8367-E035914D9D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658E5EF-4BF7-4617-9D0E-707D1DC4FC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2220" windowWidth="15600" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -42,16 +37,16 @@
     <t>Reunião com a equipe de desenvolvimento</t>
   </si>
   <si>
+    <t>Pedro</t>
+  </si>
+  <si>
     <t>Reunião com o Call Center</t>
   </si>
   <si>
+    <t>João</t>
+  </si>
+  <si>
     <t>Reunião com a Dell</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Pedro</t>
   </si>
   <si>
     <t>Maria</t>
@@ -61,13 +56,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,7 +85,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -90,16 +104,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -112,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -146,20 +179,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -189,12 +222,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -233,164 +266,191 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -400,69 +460,69 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>44911</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.72916666666666663</v>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>45350</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.91666666666666663</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>44911</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.75</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>45350</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.91666666666666663</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>44911</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.79166666666666663</v>
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45350</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.91666666666666663</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado funcionalidade de pesquisa e leitura da agenda
</commit_message>
<xml_diff>
--- a/Agenda/agenda.xlsx
+++ b/Agenda/agenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Pessoal\IA Expert\Assistente_Virtual\Agenda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Pessoal\IA_Expert\Assistente_Virtual\Agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658E5EF-4BF7-4617-9D0E-707D1DC4FC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054FF3C6-466E-418B-847C-21154C5587C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -56,19 +56,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -104,27 +98,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -435,7 +426,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +437,7 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,10 +453,10 @@
     </row>
     <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>45350</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0.91666666666666663</v>
+        <v>45362</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.91699074074074072</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -476,10 +467,10 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>45350</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.91666666666666663</v>
+        <v>45362</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.91699074074074072</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -490,10 +481,10 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>45350</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.91666666666666663</v>
+        <v>45362</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.91699074074074072</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>

</xml_diff>